<commit_message>
part of session 2
</commit_message>
<xml_diff>
--- a/data/signal-data.xlsx
+++ b/data/signal-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emi/Downloads/doi_10.5061_dryad.n50cr__v1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emi/Dropbox (Personal)/Workshops/20191201_IBSAR2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2107964C-BC79-654D-9E67-595FE21BF640}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885590A2-343C-0D46-ABA1-F083A3A6176C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,21 +69,6 @@
     <t>Frog ID</t>
   </si>
   <si>
-    <t>call duration</t>
-  </si>
-  <si>
-    <t>call rate</t>
-  </si>
-  <si>
-    <t>dominant frequency</t>
-  </si>
-  <si>
-    <t>relative amplitude</t>
-  </si>
-  <si>
-    <t>pulse rate</t>
-  </si>
-  <si>
     <t>Two Choice Latency</t>
   </si>
   <si>
@@ -97,6 +82,21 @@
   </si>
   <si>
     <t>Two Choice</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>PR</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:R536"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -431,19 +431,19 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -464,22 +464,22 @@
         <v>5</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="O1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
         <v>6</v>
       </c>
       <c r="Q1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="R1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>